<commit_message>
30 Sept 2025, penyempurnaan fitur pembayaran dan perbaikan fitur pembuatan laporan perjadin.
</commit_message>
<xml_diff>
--- a/template/Template Biaya Uang Representasi.xlsx
+++ b/template/Template Biaya Uang Representasi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Belajar Coding _Programmer\aplikasi-perjadin\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4130083E-ED56-4E60-A1D0-2F7722782C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D386C8-6976-46D9-83FD-C5F9252EB4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DEF48955-3BAF-4228-8703-FD2D8BD68B24}"/>
   </bookViews>
@@ -49,10 +49,10 @@
     <t>OH</t>
   </si>
   <si>
-    <t>PEJABAT ESELON  I</t>
-  </si>
-  <si>
-    <t>PEJABAT ESELON  II</t>
+    <t>PEJABAT ESELON II</t>
+  </si>
+  <si>
+    <t>PEJABAT ESELON I</t>
   </si>
 </sst>
 </file>
@@ -119,26 +119,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -458,7 +458,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -471,78 +471,78 @@
     <col min="8" max="8" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="42.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="28.5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="56">
-      <c r="A2" s="6">
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" ht="28">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="7">
         <v>250000</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="7">
         <v>125000</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="28">
-      <c r="A3" s="6">
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>200000</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>100000</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="28">
-      <c r="A4" s="6">
+    <row r="4" spans="1:8">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>150000</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>75000</v>
       </c>
     </row>

</xml_diff>